<commit_message>
Updated Projecttext and ProjectPlan
</commit_message>
<xml_diff>
--- a/doc/IP5_project_plan.xlsx
+++ b/doc/IP5_project_plan.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="45C1CC58B5362C6FCD129DE922EA08F0CBBED421" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E04001AC-6028-41D8-9F2F-84636AB4F0CB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -153,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +191,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -283,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -300,16 +307,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -599,24 +607,24 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="3" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +680,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>43002</v>
       </c>
@@ -728,78 +736,82 @@
         <v>43119</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="L3" s="22"/>
       <c r="R3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="F5" s="21"/>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="H6" s="21"/>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="J8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L8" s="21"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E10" s="18" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="E10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="Q10" s="16" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
+      <c r="Q10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="16"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E11" s="7" t="s">
         <v>26</v>
       </c>
@@ -811,7 +823,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E12" s="11"/>
       <c r="F12" s="8" t="s">
         <v>29</v>
@@ -823,7 +835,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -835,7 +847,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -847,19 +859,19 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="18" spans="11:18" x14ac:dyDescent="0.3">
-      <c r="K18" s="18" t="s">
+    <row r="18" spans="11:18" x14ac:dyDescent="0.45">
+      <c r="K18" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="20"/>
-    </row>
-    <row r="19" spans="11:18" x14ac:dyDescent="0.3">
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="18"/>
+    </row>
+    <row r="19" spans="11:18" x14ac:dyDescent="0.45">
       <c r="K19" s="7" t="s">
         <v>26</v>
       </c>
@@ -871,9 +883,9 @@
       <c r="Q19" s="9"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="11:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="11:18" x14ac:dyDescent="0.45">
       <c r="K20" s="11"/>
-      <c r="L20" s="21" t="s">
+      <c r="L20" s="19" t="s">
         <v>34</v>
       </c>
       <c r="M20" s="8"/>
@@ -883,7 +895,7 @@
       <c r="Q20" s="9"/>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="11:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="11:18" x14ac:dyDescent="0.45">
       <c r="K21" s="11"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
@@ -895,7 +907,7 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="11:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="11:18" x14ac:dyDescent="0.45">
       <c r="K22" s="12"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>

</xml_diff>

<commit_message>
Refactored code, moved unsused files, created tmp dir, changed import statements
</commit_message>
<xml_diff>
--- a/doc/IP5_project_plan.xlsx
+++ b/doc/IP5_project_plan.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="E708F7476A8FCD9F2B3827E86A53CE31EEC2684B" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -595,25 +596,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="3" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="18" width="10.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>43002</v>
       </c>
@@ -725,13 +726,13 @@
         <v>43119</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="L3" s="19"/>
       <c r="R3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="21" t="s">
         <v>25</v>
       </c>
@@ -740,7 +741,7 @@
       <c r="D4" s="21"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
@@ -750,7 +751,7 @@
       <c r="F5" s="21"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
@@ -760,7 +761,7 @@
       <c r="H6" s="21"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="H7" s="5" t="s">
         <v>20</v>
       </c>
@@ -769,7 +770,7 @@
       </c>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="J8" s="5" t="s">
         <v>20</v>
       </c>
@@ -778,13 +779,13 @@
       </c>
       <c r="L8" s="21"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E10" s="16" t="s">
         <v>28</v>
       </c>
@@ -800,7 +801,7 @@
       </c>
       <c r="R10" s="20"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E11" s="7" t="s">
         <v>26</v>
       </c>
@@ -812,7 +813,7 @@
       <c r="K11" s="9"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E12" s="11"/>
       <c r="F12" s="8" t="s">
         <v>27</v>
@@ -824,7 +825,7 @@
       <c r="K12" s="9"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -836,7 +837,7 @@
       <c r="K13" s="8"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -848,7 +849,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="15"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="M15" s="17" t="s">
         <v>31</v>
       </c>

</xml_diff>